<commit_message>
update with jan 2020 data
</commit_message>
<xml_diff>
--- a/Oyster/transect/data/field_schedule_Sept2019_Mar2020.xlsx
+++ b/Oyster/transect/data/field_schedule_Sept2019_Mar2020.xlsx
@@ -12869,7 +12869,7 @@
   <dimension ref="A1:J226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -20120,8 +20120,8 @@
   <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P42" sqref="P42"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>